<commit_message>
Solved naming issues in fct_check_data2 and calculations issues with formula including DG_ratio
</commit_message>
<xml_diff>
--- a/inst/extdata/example1-4pools.xlsx
+++ b/inst/extdata/example1-4pools.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaelsola/Github-Collabs/mocaredd/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ACDD24-53A2-EF4A-BE82-40D90BF45743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC83025B-AD59-1145-A8AE-F835164BAF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="760" windowWidth="28660" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,19 +418,19 @@
     <t>trans_placeholder</t>
   </si>
   <si>
-    <t>trans_lu_initial_id</t>
-  </si>
-  <si>
-    <t>trans_lu_final_id</t>
-  </si>
-  <si>
-    <t>trans_lu_initial</t>
-  </si>
-  <si>
-    <t>trans_lu_final</t>
-  </si>
-  <si>
-    <t>trans_redd_activity</t>
+    <t>lu_initial_id</t>
+  </si>
+  <si>
+    <t>lu_final_id</t>
+  </si>
+  <si>
+    <t>lu_initial</t>
+  </si>
+  <si>
+    <t>lu_final</t>
+  </si>
+  <si>
+    <t>redd_activity</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScale="186" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1230,7 +1230,7 @@
   </sheetPr>
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="127" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -1239,7 +1239,7 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -3230,7 +3230,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3240,7 +3240,7 @@
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>

</xml_diff>